<commit_message>
reworked xls import to work with categorties, added superuser creation
</commit_message>
<xml_diff>
--- a/baloons/static/import_balloons.xlsx
+++ b/baloons/static/import_balloons.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\NORS\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\PyLearning\django\baloons\static\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E0F4E7FC-22F8-48A1-8D6A-E464E02D925F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{93942E83-BF8F-45D9-AA3A-8AFAAFDB8C45}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4290" yWindow="1605" windowWidth="25620" windowHeight="12180" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2175" yWindow="2385" windowWidth="25620" windowHeight="12180" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Лист1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="16">
   <si>
     <t>name</t>
   </si>
@@ -67,6 +67,12 @@
   </si>
   <si>
     <t>products_images/8-686x1024-1-768x768.jpg</t>
+  </si>
+  <si>
+    <t>Золотой шар</t>
+  </si>
+  <si>
+    <t>Золотой шаврик</t>
   </si>
 </sst>
 </file>
@@ -387,7 +393,7 @@
   <dimension ref="A1:G3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="G14" sqref="G14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -441,8 +447,8 @@
       <c r="F2">
         <v>5</v>
       </c>
-      <c r="G2">
-        <v>1</v>
+      <c r="G2" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
@@ -464,8 +470,8 @@
       <c r="F3">
         <v>22</v>
       </c>
-      <c r="G3">
-        <v>1</v>
+      <c r="G3" t="s">
+        <v>15</v>
       </c>
     </row>
   </sheetData>

</xml_diff>